<commit_message>
Add refineryData, refineryMain, dataOut ignore
</commit_message>
<xml_diff>
--- a/refinery/data on petroleum emission for ANN.xlsx
+++ b/refinery/data on petroleum emission for ANN.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a3914e3c06405e1/Documents/CU/Collaboration/4/m1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokel\source\repos\cu\refinery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{81960107-659E-4576-9CAC-46B20C39598C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BE660F82-039C-489E-8573-EB9D8A1865D5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9365F5D0-2C26-415C-8F83-BF8FD6F3D9C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{6E5467E8-6820-4C90-9069-193058ED449C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{6E5467E8-6820-4C90-9069-193058ED449C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="116">
   <si>
     <r>
       <t>S/N</t>
@@ -542,12 +543,85 @@
   <si>
     <t xml:space="preserve">590.95 2930.4 </t>
   </si>
+  <si>
+    <t>Discharge Temp</t>
+  </si>
+  <si>
+    <t>Exit Velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release Height </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO2 </t>
+  </si>
+  <si>
+    <r>
+      <t>NO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">X </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Flare1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heater1 </t>
+  </si>
+  <si>
+    <t>Flare1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boiler1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heater1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flare2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heater2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boiler2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00322.3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flare3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boiler3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flare4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boiler4 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,6 +701,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -680,10 +776,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -791,8 +888,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -803,29 +912,55 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1140,40 +1275,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0A16BA-A2CA-4FDA-AB38-ECBAF3FF4344}">
   <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="41" t="s">
+    <row r="2" spans="1:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="47"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
+    <row r="3" spans="1:11" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1184,7 +1319,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1204,7 +1339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -1224,7 +1359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -1244,7 +1379,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -1264,7 +1399,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
         <v>5</v>
       </c>
@@ -1284,16 +1419,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="39" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1305,20 +1440,20 @@
       <c r="E10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="39" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="44" t="s">
+      <c r="I10" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="44"/>
+      <c r="J10" s="46"/>
       <c r="K10" s="35"/>
     </row>
-    <row r="11" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
-      <c r="B11" s="42"/>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1328,18 +1463,18 @@
       <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="42"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="36"/>
       <c r="H11" s="36"/>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="36"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="43"/>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="44"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="17" t="s">
         <v>18</v>
       </c>
@@ -1349,7 +1484,7 @@
       <c r="E12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="43"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="18" t="s">
         <v>27</v>
       </c>
@@ -1366,7 +1501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
@@ -1401,7 +1536,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>30</v>
       </c>
@@ -1436,7 +1571,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
@@ -1471,7 +1606,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>32</v>
       </c>
@@ -1506,7 +1641,7 @@
         <v>1510.4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -1541,7 +1676,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="20"/>
       <c r="B18" s="11" t="s">
         <v>39</v>
@@ -1574,7 +1709,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="20"/>
       <c r="B19" s="21" t="s">
         <v>40</v>
@@ -1589,7 +1724,7 @@
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="20"/>
       <c r="B20" s="11" t="s">
         <v>41</v>
@@ -1604,7 +1739,7 @@
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="23"/>
       <c r="B21" s="11" t="s">
         <v>42</v>
@@ -1637,7 +1772,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="23"/>
       <c r="B22" s="21" t="s">
         <v>43</v>
@@ -1670,7 +1805,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="23"/>
       <c r="B23" s="11" t="s">
         <v>44</v>
@@ -1703,7 +1838,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>45</v>
       </c>
@@ -1738,7 +1873,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>46</v>
       </c>
@@ -1773,7 +1908,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>47</v>
       </c>
@@ -1808,7 +1943,7 @@
         <v>347.7</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>48</v>
       </c>
@@ -1843,7 +1978,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>49</v>
       </c>
@@ -1878,7 +2013,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="20"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
@@ -1893,7 +2028,7 @@
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="23"/>
       <c r="B30" s="21" t="s">
         <v>43</v>
@@ -1926,7 +2061,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="23"/>
       <c r="B31" s="11" t="s">
         <v>44</v>
@@ -1959,7 +2094,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>45</v>
       </c>
@@ -1994,7 +2129,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>51</v>
       </c>
@@ -2029,7 +2164,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>52</v>
       </c>
@@ -2064,7 +2199,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>48</v>
       </c>
@@ -2099,7 +2234,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>53</v>
       </c>
@@ -2134,7 +2269,7 @@
         <v>2877</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="20"/>
       <c r="B37" s="21" t="s">
         <v>38</v>
@@ -2167,7 +2302,7 @@
         <v>93.4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="20"/>
       <c r="B38" s="11" t="s">
         <v>39</v>
@@ -2198,7 +2333,7 @@
         <v>93.4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="20"/>
       <c r="B39" s="21" t="s">
         <v>40</v>
@@ -2213,7 +2348,7 @@
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="20"/>
       <c r="B40" s="11" t="s">
         <v>41</v>
@@ -2228,7 +2363,7 @@
       <c r="J40" s="22"/>
       <c r="K40" s="22"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="23"/>
       <c r="B41" s="21" t="s">
         <v>40</v>
@@ -2261,7 +2396,7 @@
         <v>93.4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="23"/>
       <c r="B42" s="11" t="s">
         <v>41</v>
@@ -2294,7 +2429,7 @@
         <v>93.4</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="23"/>
       <c r="B43" s="21" t="s">
         <v>43</v>
@@ -2327,7 +2462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="24"/>
       <c r="B44" s="25" t="s">
         <v>44</v>
@@ -2360,7 +2495,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>59</v>
       </c>
@@ -2395,7 +2530,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>30</v>
       </c>
@@ -2430,7 +2565,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>31</v>
       </c>
@@ -2465,7 +2600,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>60</v>
       </c>
@@ -2500,7 +2635,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>61</v>
       </c>
@@ -2535,7 +2670,7 @@
         <v>1870.1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="20"/>
       <c r="B50" s="21" t="s">
         <v>38</v>
@@ -2568,7 +2703,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="20"/>
       <c r="B51" s="11" t="s">
         <v>39</v>
@@ -2601,7 +2736,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="20"/>
       <c r="B52" s="21" t="s">
         <v>40</v>
@@ -2616,7 +2751,7 @@
       <c r="J52" s="22"/>
       <c r="K52" s="22"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="20"/>
       <c r="B53" s="11" t="s">
         <v>41</v>
@@ -2631,7 +2766,7 @@
       <c r="J53" s="22"/>
       <c r="K53" s="22"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="23"/>
       <c r="B54" s="11" t="s">
         <v>42</v>
@@ -2664,7 +2799,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="23"/>
       <c r="B55" s="21" t="s">
         <v>43</v>
@@ -2697,7 +2832,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="23"/>
       <c r="B56" s="11" t="s">
         <v>44</v>
@@ -2730,16 +2865,16 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="39" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -2751,20 +2886,20 @@
       <c r="E59" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F59" s="41" t="s">
+      <c r="F59" s="39" t="s">
         <v>24</v>
       </c>
       <c r="G59" s="35"/>
       <c r="H59" s="35"/>
-      <c r="I59" s="44" t="s">
+      <c r="I59" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="J59" s="44"/>
+      <c r="J59" s="46"/>
       <c r="K59" s="35"/>
     </row>
-    <row r="60" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="39"/>
-      <c r="B60" s="42"/>
+    <row r="60" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="43"/>
+      <c r="B60" s="45"/>
       <c r="C60" s="1" t="s">
         <v>17</v>
       </c>
@@ -2774,18 +2909,18 @@
       <c r="E60" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="42"/>
+      <c r="F60" s="45"/>
       <c r="G60" s="36"/>
       <c r="H60" s="36"/>
-      <c r="I60" s="43" t="s">
+      <c r="I60" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="43"/>
+      <c r="J60" s="40"/>
       <c r="K60" s="36"/>
     </row>
-    <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="40"/>
-      <c r="B61" s="43"/>
+    <row r="61" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="44"/>
+      <c r="B61" s="40"/>
       <c r="C61" s="17" t="s">
         <v>18</v>
       </c>
@@ -2795,7 +2930,7 @@
       <c r="E61" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F61" s="43"/>
+      <c r="F61" s="40"/>
       <c r="G61" s="18" t="s">
         <v>27</v>
       </c>
@@ -2812,7 +2947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
         <v>63</v>
       </c>
@@ -2847,7 +2982,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>64</v>
       </c>
@@ -2882,7 +3017,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
         <v>65</v>
       </c>
@@ -2917,7 +3052,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>66</v>
       </c>
@@ -2952,7 +3087,7 @@
         <v>965.9</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="20"/>
       <c r="B66" s="21" t="s">
         <v>38</v>
@@ -2985,7 +3120,7 @@
         <v>57.8</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="20"/>
       <c r="B67" s="11" t="s">
         <v>39</v>
@@ -3018,7 +3153,7 @@
         <v>57.8</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="20"/>
       <c r="B68" s="21" t="s">
         <v>40</v>
@@ -3033,7 +3168,7 @@
       <c r="J68" s="22"/>
       <c r="K68" s="22"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="20"/>
       <c r="B69" s="11" t="s">
         <v>41</v>
@@ -3048,7 +3183,7 @@
       <c r="J69" s="22"/>
       <c r="K69" s="22"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="23"/>
       <c r="B70" s="21" t="s">
         <v>43</v>
@@ -3081,7 +3216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="23"/>
       <c r="B71" s="11" t="s">
         <v>44</v>
@@ -3114,7 +3249,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
         <v>67</v>
       </c>
@@ -3149,7 +3284,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>68</v>
       </c>
@@ -3184,7 +3319,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
         <v>69</v>
       </c>
@@ -3219,7 +3354,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>70</v>
       </c>
@@ -3254,7 +3389,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="20"/>
       <c r="B76" s="11" t="s">
         <v>54</v>
@@ -3287,7 +3422,7 @@
         <v>1390.9</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="20"/>
       <c r="B77" s="21" t="s">
         <v>38</v>
@@ -3318,7 +3453,7 @@
         <v>83.2</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="20"/>
       <c r="B78" s="11" t="s">
         <v>39</v>
@@ -3333,7 +3468,7 @@
       <c r="J78" s="22"/>
       <c r="K78" s="22"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="20"/>
       <c r="B79" s="21" t="s">
         <v>40</v>
@@ -3348,7 +3483,7 @@
       <c r="J79" s="22"/>
       <c r="K79" s="22"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="23"/>
       <c r="B80" s="11" t="s">
         <v>41</v>
@@ -3381,7 +3516,7 @@
         <v>83.2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="23"/>
       <c r="B81" s="21" t="s">
         <v>43</v>
@@ -3414,7 +3549,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="23"/>
       <c r="B82" s="11" t="s">
         <v>44</v>
@@ -3447,7 +3582,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="10" t="s">
         <v>72</v>
       </c>
@@ -3482,7 +3617,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A84" s="11" t="s">
         <v>73</v>
       </c>
@@ -3517,7 +3652,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
         <v>74</v>
       </c>
@@ -3552,7 +3687,7 @@
         <v>347.7</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="20"/>
       <c r="B86" s="11" t="s">
         <v>39</v>
@@ -3583,7 +3718,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="20"/>
       <c r="B87" s="21" t="s">
         <v>40</v>
@@ -3598,7 +3733,7 @@
       <c r="J87" s="30"/>
       <c r="K87" s="30"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="23"/>
       <c r="B88" s="11" t="s">
         <v>41</v>
@@ -3631,7 +3766,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="23"/>
       <c r="B89" s="21" t="s">
         <v>43</v>
@@ -3664,7 +3799,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="24"/>
       <c r="B90" s="25" t="s">
         <v>44</v>
@@ -3697,7 +3832,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>76</v>
       </c>
@@ -3732,7 +3867,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A92" s="11" t="s">
         <v>77</v>
       </c>
@@ -3767,7 +3902,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="11" t="s">
         <v>78</v>
       </c>
@@ -3802,7 +3937,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="11" t="s">
         <v>45</v>
       </c>
@@ -3837,7 +3972,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="11" t="s">
         <v>79</v>
       </c>
@@ -3870,7 +4005,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="20"/>
       <c r="B96" s="11" t="s">
         <v>41</v>
@@ -3885,7 +4020,7 @@
       <c r="J96" s="22"/>
       <c r="K96" s="22"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="23"/>
       <c r="B97" s="21" t="s">
         <v>43</v>
@@ -3918,7 +4053,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="23"/>
       <c r="B98" s="11" t="s">
         <v>44</v>
@@ -3951,7 +4086,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="7" t="s">
         <v>80</v>
       </c>
@@ -3986,7 +4121,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="7" t="s">
         <v>81</v>
       </c>
@@ -4021,7 +4156,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="11" t="s">
         <v>82</v>
       </c>
@@ -4056,7 +4191,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="20"/>
       <c r="B102" s="11" t="s">
         <v>37</v>
@@ -4089,7 +4224,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="20"/>
       <c r="B103" s="11" t="s">
         <v>54</v>
@@ -4122,7 +4257,7 @@
         <v>60006</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="20"/>
       <c r="B104" s="21" t="s">
         <v>38</v>
@@ -4155,7 +4290,7 @@
         <v>8033.4</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="20"/>
       <c r="B105" s="11" t="s">
         <v>39</v>
@@ -4170,7 +4305,7 @@
       <c r="J105" s="22"/>
       <c r="K105" s="22"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="20"/>
       <c r="B106" s="21" t="s">
         <v>40</v>
@@ -4185,7 +4320,7 @@
       <c r="J106" s="22"/>
       <c r="K106" s="22"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="23"/>
       <c r="B107" s="11" t="s">
         <v>41</v>
@@ -4218,7 +4353,7 @@
         <v>8033.4</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="23"/>
       <c r="B108" s="11" t="s">
         <v>42</v>
@@ -4251,7 +4386,7 @@
         <v>8033.4</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="23"/>
       <c r="B109" s="11" t="s">
         <v>83</v>
@@ -4284,7 +4419,7 @@
         <v>8033.4</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="23"/>
       <c r="B110" s="21" t="s">
         <v>43</v>
@@ -4317,7 +4452,7 @@
         <v>1811.1</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="23"/>
       <c r="B111" s="11" t="s">
         <v>44</v>
@@ -4350,7 +4485,7 @@
         <v>1811.1</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="8" t="s">
         <v>84</v>
       </c>
@@ -4385,7 +4520,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A113" s="7" t="s">
         <v>85</v>
       </c>
@@ -4420,7 +4555,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" s="7" t="s">
         <v>63</v>
       </c>
@@ -4455,7 +4590,7 @@
         <v>10167</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" s="7" t="s">
         <v>86</v>
       </c>
@@ -4490,7 +4625,7 @@
         <v>608.33000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" s="34">
         <v>55000</v>
       </c>
@@ -4525,7 +4660,7 @@
         <v>608.33000000000004</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" s="8" t="s">
         <v>87</v>
       </c>
@@ -4542,7 +4677,7 @@
       <c r="J117" s="22"/>
       <c r="K117" s="22"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="23"/>
       <c r="B118" s="21" t="s">
         <v>43</v>
@@ -4575,7 +4710,7 @@
         <v>139.05000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="23"/>
       <c r="B119" s="11" t="s">
         <v>44</v>
@@ -4608,7 +4743,7 @@
         <v>139.05000000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" s="7" t="s">
         <v>88</v>
       </c>
@@ -4627,7 +4762,7 @@
       <c r="F120" s="11">
         <v>7</v>
       </c>
-      <c r="G120" s="37"/>
+      <c r="G120" s="47"/>
       <c r="H120" s="7" t="s">
         <v>9</v>
       </c>
@@ -4641,7 +4776,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A121" s="7" t="s">
         <v>89</v>
       </c>
@@ -4660,7 +4795,7 @@
       <c r="F121" s="11">
         <v>7</v>
       </c>
-      <c r="G121" s="37"/>
+      <c r="G121" s="47"/>
       <c r="H121" s="7" t="s">
         <v>9</v>
       </c>
@@ -4674,7 +4809,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" s="7" t="s">
         <v>81</v>
       </c>
@@ -4693,7 +4828,7 @@
       <c r="F122" s="11">
         <v>7</v>
       </c>
-      <c r="G122" s="37"/>
+      <c r="G122" s="47"/>
       <c r="H122" s="11">
         <v>13.7</v>
       </c>
@@ -4707,7 +4842,7 @@
         <v>483.19</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" s="11" t="s">
         <v>90</v>
       </c>
@@ -4726,7 +4861,7 @@
       <c r="F123" s="11">
         <v>3</v>
       </c>
-      <c r="G123" s="37"/>
+      <c r="G123" s="47"/>
       <c r="H123" s="11">
         <v>560.04999999999995</v>
       </c>
@@ -4740,7 +4875,7 @@
         <v>209.24</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" s="20"/>
       <c r="B124" s="21" t="s">
         <v>40</v>
@@ -4757,7 +4892,7 @@
       <c r="F124" s="11">
         <v>3</v>
       </c>
-      <c r="G124" s="37"/>
+      <c r="G124" s="47"/>
       <c r="H124" s="11">
         <v>560.04999999999995</v>
       </c>
@@ -4771,7 +4906,7 @@
         <v>209.24</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" s="20"/>
       <c r="B125" s="11" t="s">
         <v>41</v>
@@ -4780,13 +4915,13 @@
       <c r="D125" s="22"/>
       <c r="E125" s="22"/>
       <c r="F125" s="22"/>
-      <c r="G125" s="37"/>
+      <c r="G125" s="47"/>
       <c r="H125" s="22"/>
       <c r="I125" s="22"/>
       <c r="J125" s="22"/>
       <c r="K125" s="22"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" s="23"/>
       <c r="B126" s="21" t="s">
         <v>43</v>
@@ -4819,7 +4954,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" s="23"/>
       <c r="B127" s="11" t="s">
         <v>44</v>
@@ -4852,7 +4987,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" s="7" t="s">
         <v>91</v>
       </c>
@@ -4887,7 +5022,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
         <v>92</v>
       </c>
@@ -4922,7 +5057,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A130" s="11" t="s">
         <v>93</v>
       </c>
@@ -4957,7 +5092,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="8" t="s">
         <v>94</v>
       </c>
@@ -4992,7 +5127,7 @@
         <v>983.8</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" s="20"/>
       <c r="B132" s="21" t="s">
         <v>40</v>
@@ -5021,7 +5156,7 @@
         <v>983.8</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" s="20"/>
       <c r="B133" s="11" t="s">
         <v>41</v>
@@ -5036,7 +5171,7 @@
       <c r="J133" s="22"/>
       <c r="K133" s="22"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" s="23"/>
       <c r="B134" s="21" t="s">
         <v>43</v>
@@ -5069,7 +5204,7 @@
         <v>222.48</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" s="23"/>
       <c r="B135" s="11" t="s">
         <v>44</v>
@@ -5104,6 +5239,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="K59:K60"/>
+    <mergeCell ref="G120:G125"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -5116,17 +5260,2479 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K59:K60"/>
-    <mergeCell ref="G120:G125"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="I60:J60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5EEE48-A2E5-43AD-A3CE-1A050819C165}">
+  <dimension ref="A1:J77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:J77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="48"/>
+    <col min="2" max="2" width="15.90625" style="48" customWidth="1"/>
+    <col min="3" max="4" width="8.7265625" style="48"/>
+    <col min="5" max="5" width="11.08984375" style="48" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="8.7265625" style="48"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="55">
+        <v>1540</v>
+      </c>
+      <c r="C2" s="57">
+        <v>6.6</v>
+      </c>
+      <c r="D2" s="57">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="E2" s="57">
+        <v>66</v>
+      </c>
+      <c r="F2" s="57">
+        <v>0</v>
+      </c>
+      <c r="G2" s="57">
+        <v>0</v>
+      </c>
+      <c r="H2" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I2" s="57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J2" s="57">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="55">
+        <v>1540</v>
+      </c>
+      <c r="C3" s="57">
+        <v>6.6</v>
+      </c>
+      <c r="D3" s="57">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="E3" s="57">
+        <v>66</v>
+      </c>
+      <c r="F3" s="57">
+        <v>0</v>
+      </c>
+      <c r="G3" s="57">
+        <v>0</v>
+      </c>
+      <c r="H3" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I3" s="57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J3" s="57">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="55">
+        <v>330</v>
+      </c>
+      <c r="C4" s="57">
+        <v>2.75</v>
+      </c>
+      <c r="D4" s="57">
+        <v>23.47</v>
+      </c>
+      <c r="E4" s="57">
+        <v>67</v>
+      </c>
+      <c r="F4" s="57">
+        <v>0</v>
+      </c>
+      <c r="G4" s="57">
+        <v>54.5</v>
+      </c>
+      <c r="H4" s="57">
+        <v>7.9</v>
+      </c>
+      <c r="I4" s="57">
+        <v>24.3</v>
+      </c>
+      <c r="J4" s="57">
+        <v>1510.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="55">
+        <v>550</v>
+      </c>
+      <c r="C5" s="57">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D5" s="57">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="E5" s="57">
+        <v>30</v>
+      </c>
+      <c r="F5" s="57">
+        <v>0</v>
+      </c>
+      <c r="G5" s="57">
+        <v>304.10000000000002</v>
+      </c>
+      <c r="H5" s="57">
+        <v>1420.1</v>
+      </c>
+      <c r="I5" s="57">
+        <v>0</v>
+      </c>
+      <c r="J5" s="57">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="55">
+        <v>550</v>
+      </c>
+      <c r="C6" s="57">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D6" s="57">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="E6" s="57">
+        <v>30</v>
+      </c>
+      <c r="F6" s="57">
+        <v>0</v>
+      </c>
+      <c r="G6" s="57">
+        <v>304.10000000000002</v>
+      </c>
+      <c r="H6" s="57">
+        <v>1420.1</v>
+      </c>
+      <c r="I6" s="57">
+        <v>0</v>
+      </c>
+      <c r="J6" s="57">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="55">
+        <v>660</v>
+      </c>
+      <c r="C7" s="57">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D7" s="57">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="E7" s="57">
+        <v>43</v>
+      </c>
+      <c r="F7" s="57">
+        <v>2.1</v>
+      </c>
+      <c r="G7" s="57">
+        <v>45.1</v>
+      </c>
+      <c r="H7" s="57">
+        <v>173.2</v>
+      </c>
+      <c r="I7" s="57">
+        <v>1</v>
+      </c>
+      <c r="J7" s="57">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="55">
+        <v>660</v>
+      </c>
+      <c r="C8" s="57">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D8" s="57">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="E8" s="57">
+        <v>43</v>
+      </c>
+      <c r="F8" s="57">
+        <v>2.1</v>
+      </c>
+      <c r="G8" s="57">
+        <v>45.1</v>
+      </c>
+      <c r="H8" s="57">
+        <v>173.2</v>
+      </c>
+      <c r="I8" s="57">
+        <v>1</v>
+      </c>
+      <c r="J8" s="57">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="55">
+        <v>840</v>
+      </c>
+      <c r="C9" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D9" s="57">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E9" s="57">
+        <v>36</v>
+      </c>
+      <c r="F9" s="57">
+        <v>0</v>
+      </c>
+      <c r="G9" s="57">
+        <v>0</v>
+      </c>
+      <c r="H9" s="57">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="I9" s="57">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="J9" s="57">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="55">
+        <v>300</v>
+      </c>
+      <c r="C10" s="57">
+        <v>1.19</v>
+      </c>
+      <c r="D10" s="57">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E10" s="57">
+        <v>16</v>
+      </c>
+      <c r="F10" s="57">
+        <v>0</v>
+      </c>
+      <c r="G10" s="57">
+        <v>59.6</v>
+      </c>
+      <c r="H10" s="57">
+        <v>278.7</v>
+      </c>
+      <c r="I10" s="57">
+        <v>0</v>
+      </c>
+      <c r="J10" s="57">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="55">
+        <v>300</v>
+      </c>
+      <c r="C11" s="57">
+        <v>1.19</v>
+      </c>
+      <c r="D11" s="57">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E11" s="57">
+        <v>16</v>
+      </c>
+      <c r="F11" s="57">
+        <v>0</v>
+      </c>
+      <c r="G11" s="57">
+        <v>59.6</v>
+      </c>
+      <c r="H11" s="57">
+        <v>278.7</v>
+      </c>
+      <c r="I11" s="57">
+        <v>0</v>
+      </c>
+      <c r="J11" s="57">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="55">
+        <v>360</v>
+      </c>
+      <c r="C12" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D12" s="57">
+        <v>4.38</v>
+      </c>
+      <c r="E12" s="57">
+        <v>24</v>
+      </c>
+      <c r="F12" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="G12" s="57">
+        <v>13.4</v>
+      </c>
+      <c r="H12" s="57">
+        <v>51.6</v>
+      </c>
+      <c r="I12" s="57">
+        <v>0.3</v>
+      </c>
+      <c r="J12" s="57">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="55">
+        <v>360</v>
+      </c>
+      <c r="C13" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D13" s="57">
+        <v>4.38</v>
+      </c>
+      <c r="E13" s="57">
+        <v>24</v>
+      </c>
+      <c r="F13" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="G13" s="57">
+        <v>13.4</v>
+      </c>
+      <c r="H13" s="57">
+        <v>51.6</v>
+      </c>
+      <c r="I13" s="57">
+        <v>0.3</v>
+      </c>
+      <c r="J13" s="57">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="55">
+        <v>2100</v>
+      </c>
+      <c r="C14" s="57">
+        <v>2.75</v>
+      </c>
+      <c r="D14" s="57">
+        <v>6.17</v>
+      </c>
+      <c r="E14" s="57">
+        <v>90</v>
+      </c>
+      <c r="F14" s="57">
+        <v>0</v>
+      </c>
+      <c r="G14" s="57">
+        <v>0</v>
+      </c>
+      <c r="H14" s="57">
+        <v>2E-3</v>
+      </c>
+      <c r="I14" s="57">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J14" s="57">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="55">
+        <v>2100</v>
+      </c>
+      <c r="C15" s="57">
+        <v>2.75</v>
+      </c>
+      <c r="D15" s="57">
+        <v>6.17</v>
+      </c>
+      <c r="E15" s="57">
+        <v>90</v>
+      </c>
+      <c r="F15" s="57">
+        <v>0</v>
+      </c>
+      <c r="G15" s="57">
+        <v>0</v>
+      </c>
+      <c r="H15" s="57">
+        <v>2E-3</v>
+      </c>
+      <c r="I15" s="57">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J15" s="57">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="55">
+        <v>2100</v>
+      </c>
+      <c r="C16" s="57">
+        <v>2.75</v>
+      </c>
+      <c r="D16" s="57">
+        <v>6.17</v>
+      </c>
+      <c r="E16" s="57">
+        <v>90</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="57">
+        <v>2E-3</v>
+      </c>
+      <c r="I16" s="57">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J16" s="57">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="55">
+        <v>450</v>
+      </c>
+      <c r="C17" s="57">
+        <v>3.75</v>
+      </c>
+      <c r="D17" s="57">
+        <v>32.01</v>
+      </c>
+      <c r="E17" s="57">
+        <v>92</v>
+      </c>
+      <c r="F17" s="57">
+        <v>0</v>
+      </c>
+      <c r="G17" s="57">
+        <v>103.5</v>
+      </c>
+      <c r="H17" s="57">
+        <v>14.9</v>
+      </c>
+      <c r="I17" s="57">
+        <v>0</v>
+      </c>
+      <c r="J17" s="57">
+        <v>2877</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="55">
+        <v>750</v>
+      </c>
+      <c r="C18" s="57">
+        <v>2.97</v>
+      </c>
+      <c r="D18" s="57">
+        <v>12.35</v>
+      </c>
+      <c r="E18" s="57">
+        <v>41</v>
+      </c>
+      <c r="F18" s="57">
+        <v>0</v>
+      </c>
+      <c r="G18" s="57">
+        <v>267.8</v>
+      </c>
+      <c r="H18" s="57">
+        <v>1250.7</v>
+      </c>
+      <c r="I18" s="58"/>
+      <c r="J18" s="57">
+        <v>93.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="55">
+        <v>750</v>
+      </c>
+      <c r="C19" s="57">
+        <v>2.97</v>
+      </c>
+      <c r="D19" s="57">
+        <v>12.35</v>
+      </c>
+      <c r="E19" s="57">
+        <v>41</v>
+      </c>
+      <c r="F19" s="57">
+        <v>0</v>
+      </c>
+      <c r="G19" s="57">
+        <v>267.8</v>
+      </c>
+      <c r="H19" s="57">
+        <v>1250.7</v>
+      </c>
+      <c r="I19" s="57">
+        <v>0</v>
+      </c>
+      <c r="J19" s="57">
+        <v>93.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="55">
+        <v>750</v>
+      </c>
+      <c r="C20" s="57">
+        <v>2.97</v>
+      </c>
+      <c r="D20" s="57">
+        <v>12.35</v>
+      </c>
+      <c r="E20" s="57">
+        <v>41</v>
+      </c>
+      <c r="F20" s="57">
+        <v>0</v>
+      </c>
+      <c r="G20" s="57">
+        <v>267.8</v>
+      </c>
+      <c r="H20" s="57">
+        <v>1250.7</v>
+      </c>
+      <c r="I20" s="57">
+        <v>0</v>
+      </c>
+      <c r="J20" s="57">
+        <v>93.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="55">
+        <v>900</v>
+      </c>
+      <c r="C21" s="57">
+        <v>2.75</v>
+      </c>
+      <c r="D21" s="57">
+        <v>10.95</v>
+      </c>
+      <c r="E21" s="57">
+        <v>59</v>
+      </c>
+      <c r="F21" s="57">
+        <v>3.7</v>
+      </c>
+      <c r="G21" s="57">
+        <v>80.2</v>
+      </c>
+      <c r="H21" s="57">
+        <v>308.10000000000002</v>
+      </c>
+      <c r="I21" s="57">
+        <v>1.7</v>
+      </c>
+      <c r="J21" s="57">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="56">
+        <v>900</v>
+      </c>
+      <c r="C22" s="59">
+        <v>2.75</v>
+      </c>
+      <c r="D22" s="59">
+        <v>10.95</v>
+      </c>
+      <c r="E22" s="59">
+        <v>59</v>
+      </c>
+      <c r="F22" s="59">
+        <v>3.7</v>
+      </c>
+      <c r="G22" s="59">
+        <v>80.2</v>
+      </c>
+      <c r="H22" s="59">
+        <v>308.10000000000002</v>
+      </c>
+      <c r="I22" s="59">
+        <v>1.7</v>
+      </c>
+      <c r="J22" s="59">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="55">
+        <v>1750</v>
+      </c>
+      <c r="C23" s="57">
+        <v>2.29</v>
+      </c>
+      <c r="D23" s="57">
+        <v>5.13</v>
+      </c>
+      <c r="E23" s="57">
+        <v>75</v>
+      </c>
+      <c r="F23" s="57">
+        <v>0</v>
+      </c>
+      <c r="G23" s="57">
+        <v>0</v>
+      </c>
+      <c r="H23" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I23" s="57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J23" s="57">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="55">
+        <v>1750</v>
+      </c>
+      <c r="C24" s="57">
+        <v>2.29</v>
+      </c>
+      <c r="D24" s="57">
+        <v>5.13</v>
+      </c>
+      <c r="E24" s="57">
+        <v>75</v>
+      </c>
+      <c r="F24" s="57">
+        <v>0</v>
+      </c>
+      <c r="G24" s="57">
+        <v>0</v>
+      </c>
+      <c r="H24" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I24" s="57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J24" s="57">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="55">
+        <v>1750</v>
+      </c>
+      <c r="C25" s="57">
+        <v>2.29</v>
+      </c>
+      <c r="D25" s="57">
+        <v>5.13</v>
+      </c>
+      <c r="E25" s="57">
+        <v>75</v>
+      </c>
+      <c r="F25" s="57">
+        <v>0</v>
+      </c>
+      <c r="G25" s="57">
+        <v>0</v>
+      </c>
+      <c r="H25" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I25" s="57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J25" s="57">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="55">
+        <v>375</v>
+      </c>
+      <c r="C26" s="57">
+        <v>3.13</v>
+      </c>
+      <c r="D26" s="57">
+        <v>26.68</v>
+      </c>
+      <c r="E26" s="57">
+        <v>76</v>
+      </c>
+      <c r="F26" s="57">
+        <v>0</v>
+      </c>
+      <c r="G26" s="57">
+        <v>67.3</v>
+      </c>
+      <c r="H26" s="57">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I26" s="57">
+        <v>30</v>
+      </c>
+      <c r="J26" s="57">
+        <v>1870.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="55">
+        <v>625</v>
+      </c>
+      <c r="C27" s="57">
+        <v>2.48</v>
+      </c>
+      <c r="D27" s="57">
+        <v>10.29</v>
+      </c>
+      <c r="E27" s="57">
+        <v>34</v>
+      </c>
+      <c r="F27" s="57">
+        <v>0</v>
+      </c>
+      <c r="G27" s="57">
+        <v>228.8</v>
+      </c>
+      <c r="H27" s="57">
+        <v>1068.3</v>
+      </c>
+      <c r="I27" s="57">
+        <v>0</v>
+      </c>
+      <c r="J27" s="57">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="55">
+        <v>625</v>
+      </c>
+      <c r="C28" s="57">
+        <v>2.48</v>
+      </c>
+      <c r="D28" s="57">
+        <v>10.29</v>
+      </c>
+      <c r="E28" s="57">
+        <v>34</v>
+      </c>
+      <c r="F28" s="57">
+        <v>0</v>
+      </c>
+      <c r="G28" s="57">
+        <v>228.8</v>
+      </c>
+      <c r="H28" s="57">
+        <v>1068.3</v>
+      </c>
+      <c r="I28" s="57">
+        <v>0</v>
+      </c>
+      <c r="J28" s="57">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="55">
+        <v>750</v>
+      </c>
+      <c r="C29" s="57">
+        <v>2.29</v>
+      </c>
+      <c r="D29" s="57">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="E29" s="57">
+        <v>49</v>
+      </c>
+      <c r="F29" s="57">
+        <v>2.9</v>
+      </c>
+      <c r="G29" s="57">
+        <v>61.3</v>
+      </c>
+      <c r="H29" s="57">
+        <v>253.3</v>
+      </c>
+      <c r="I29" s="57">
+        <v>1.3</v>
+      </c>
+      <c r="J29" s="57">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="55">
+        <v>750</v>
+      </c>
+      <c r="C30" s="57">
+        <v>2.29</v>
+      </c>
+      <c r="D30" s="57">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="E30" s="57">
+        <v>49</v>
+      </c>
+      <c r="F30" s="57">
+        <v>2.9</v>
+      </c>
+      <c r="G30" s="57">
+        <v>61.3</v>
+      </c>
+      <c r="H30" s="57">
+        <v>253.3</v>
+      </c>
+      <c r="I30" s="57">
+        <v>1.3</v>
+      </c>
+      <c r="J30" s="57">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="55">
+        <v>1400</v>
+      </c>
+      <c r="C31" s="57">
+        <v>1.83</v>
+      </c>
+      <c r="D31" s="57">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="E31" s="57">
+        <v>60</v>
+      </c>
+      <c r="F31" s="57">
+        <v>0</v>
+      </c>
+      <c r="G31" s="57">
+        <v>0</v>
+      </c>
+      <c r="H31" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I31" s="57">
+        <v>2E-3</v>
+      </c>
+      <c r="J31" s="57">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="55">
+        <v>1400</v>
+      </c>
+      <c r="C32" s="57">
+        <v>1.83</v>
+      </c>
+      <c r="D32" s="57">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="E32" s="57">
+        <v>60</v>
+      </c>
+      <c r="F32" s="57">
+        <v>0</v>
+      </c>
+      <c r="G32" s="57">
+        <v>0</v>
+      </c>
+      <c r="H32" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I32" s="57">
+        <v>2E-3</v>
+      </c>
+      <c r="J32" s="57">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="55">
+        <v>300</v>
+      </c>
+      <c r="C33" s="57">
+        <v>2.5</v>
+      </c>
+      <c r="D33" s="57">
+        <v>21.34</v>
+      </c>
+      <c r="E33" s="57">
+        <v>61</v>
+      </c>
+      <c r="F33" s="57">
+        <v>0</v>
+      </c>
+      <c r="G33" s="57">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="H33" s="57">
+        <v>5</v>
+      </c>
+      <c r="I33" s="57">
+        <v>15.6</v>
+      </c>
+      <c r="J33" s="57">
+        <v>965.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="55">
+        <v>500</v>
+      </c>
+      <c r="C34" s="57">
+        <v>1.98</v>
+      </c>
+      <c r="D34" s="57">
+        <v>8.23</v>
+      </c>
+      <c r="E34" s="57">
+        <v>27</v>
+      </c>
+      <c r="F34" s="57">
+        <v>0</v>
+      </c>
+      <c r="G34" s="57">
+        <v>165.7</v>
+      </c>
+      <c r="H34" s="57">
+        <v>773.9</v>
+      </c>
+      <c r="I34" s="57">
+        <v>0</v>
+      </c>
+      <c r="J34" s="57">
+        <v>57.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="55">
+        <v>600</v>
+      </c>
+      <c r="C35" s="57">
+        <v>1.83</v>
+      </c>
+      <c r="D35" s="57">
+        <v>7.3</v>
+      </c>
+      <c r="E35" s="57">
+        <v>39</v>
+      </c>
+      <c r="F35" s="57">
+        <v>1.7</v>
+      </c>
+      <c r="G35" s="57">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="H35" s="57">
+        <v>143.19999999999999</v>
+      </c>
+      <c r="I35" s="57">
+        <v>0.8</v>
+      </c>
+      <c r="J35" s="57">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="55">
+        <v>600</v>
+      </c>
+      <c r="C36" s="57">
+        <v>1.83</v>
+      </c>
+      <c r="D36" s="57">
+        <v>7.3</v>
+      </c>
+      <c r="E36" s="57">
+        <v>39</v>
+      </c>
+      <c r="F36" s="57">
+        <v>1.7</v>
+      </c>
+      <c r="G36" s="57">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="H36" s="57">
+        <v>143.19999999999999</v>
+      </c>
+      <c r="I36" s="57">
+        <v>0.8</v>
+      </c>
+      <c r="J36" s="57">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="55">
+        <v>1680</v>
+      </c>
+      <c r="C37" s="57">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D37" s="57">
+        <v>4.93</v>
+      </c>
+      <c r="E37" s="57">
+        <v>72</v>
+      </c>
+      <c r="F37" s="57">
+        <v>0</v>
+      </c>
+      <c r="G37" s="57">
+        <v>0</v>
+      </c>
+      <c r="H37" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I37" s="57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J37" s="57">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="55">
+        <v>1680</v>
+      </c>
+      <c r="C38" s="57">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D38" s="57">
+        <v>4.93</v>
+      </c>
+      <c r="E38" s="57">
+        <v>72</v>
+      </c>
+      <c r="F38" s="57">
+        <v>0</v>
+      </c>
+      <c r="G38" s="57">
+        <v>0</v>
+      </c>
+      <c r="H38" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I38" s="57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J38" s="57">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="55">
+        <v>1680</v>
+      </c>
+      <c r="C39" s="57">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D39" s="57">
+        <v>4.93</v>
+      </c>
+      <c r="E39" s="57">
+        <v>72</v>
+      </c>
+      <c r="F39" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="G39" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I39" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="J39" s="57">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="55">
+        <v>360</v>
+      </c>
+      <c r="C40" s="57">
+        <v>3</v>
+      </c>
+      <c r="D40" s="57">
+        <v>25.61</v>
+      </c>
+      <c r="E40" s="57">
+        <v>73</v>
+      </c>
+      <c r="F40" s="57">
+        <v>0</v>
+      </c>
+      <c r="G40" s="57">
+        <v>50.1</v>
+      </c>
+      <c r="H40" s="57">
+        <v>7.1</v>
+      </c>
+      <c r="I40" s="57">
+        <v>0</v>
+      </c>
+      <c r="J40" s="57">
+        <v>1390.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="55">
+        <v>600</v>
+      </c>
+      <c r="C41" s="57">
+        <v>2.38</v>
+      </c>
+      <c r="D41" s="57">
+        <v>10</v>
+      </c>
+      <c r="E41" s="57">
+        <v>33</v>
+      </c>
+      <c r="F41" s="57">
+        <v>0</v>
+      </c>
+      <c r="G41" s="57">
+        <v>238.6</v>
+      </c>
+      <c r="H41" s="57">
+        <v>1114.4000000000001</v>
+      </c>
+      <c r="I41" s="57">
+        <v>0</v>
+      </c>
+      <c r="J41" s="57">
+        <v>83.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="55">
+        <v>720</v>
+      </c>
+      <c r="C42" s="57">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D42" s="57">
+        <v>8.76</v>
+      </c>
+      <c r="E42" s="57">
+        <v>47</v>
+      </c>
+      <c r="F42" s="57">
+        <v>2.5</v>
+      </c>
+      <c r="G42" s="57">
+        <v>53.7</v>
+      </c>
+      <c r="H42" s="57">
+        <v>206.1</v>
+      </c>
+      <c r="I42" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J42" s="57">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="55">
+        <v>720</v>
+      </c>
+      <c r="C43" s="57">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D43" s="57">
+        <v>8.76</v>
+      </c>
+      <c r="E43" s="57">
+        <v>47</v>
+      </c>
+      <c r="F43" s="57">
+        <v>2.5</v>
+      </c>
+      <c r="G43" s="57">
+        <v>53.7</v>
+      </c>
+      <c r="H43" s="57">
+        <v>206.1</v>
+      </c>
+      <c r="I43" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J43" s="57">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="55">
+        <v>840</v>
+      </c>
+      <c r="C44" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D44" s="57">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E44" s="57">
+        <v>36</v>
+      </c>
+      <c r="F44" s="57">
+        <v>0</v>
+      </c>
+      <c r="G44" s="57">
+        <v>0</v>
+      </c>
+      <c r="H44" s="57">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="I44" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="J44" s="57">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="55">
+        <v>300</v>
+      </c>
+      <c r="C45" s="57">
+        <v>1.19</v>
+      </c>
+      <c r="D45" s="57">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E45" s="57">
+        <v>16</v>
+      </c>
+      <c r="F45" s="57">
+        <v>0</v>
+      </c>
+      <c r="G45" s="57">
+        <v>59.6</v>
+      </c>
+      <c r="H45" s="57">
+        <v>278.7</v>
+      </c>
+      <c r="I45" s="60"/>
+      <c r="J45" s="57">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="55">
+        <v>300</v>
+      </c>
+      <c r="C46" s="57">
+        <v>1.19</v>
+      </c>
+      <c r="D46" s="57">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E46" s="57">
+        <v>16</v>
+      </c>
+      <c r="F46" s="57">
+        <v>0</v>
+      </c>
+      <c r="G46" s="57">
+        <v>59.6</v>
+      </c>
+      <c r="H46" s="57">
+        <v>278.7</v>
+      </c>
+      <c r="I46" s="57">
+        <v>0</v>
+      </c>
+      <c r="J46" s="57">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="55">
+        <v>360</v>
+      </c>
+      <c r="C47" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D47" s="57">
+        <v>4.38</v>
+      </c>
+      <c r="E47" s="57">
+        <v>24</v>
+      </c>
+      <c r="F47" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="G47" s="57">
+        <v>13.4</v>
+      </c>
+      <c r="H47" s="57">
+        <v>51.6</v>
+      </c>
+      <c r="I47" s="57">
+        <v>0.3</v>
+      </c>
+      <c r="J47" s="57">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="56">
+        <v>360</v>
+      </c>
+      <c r="C48" s="59">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D48" s="59">
+        <v>4.38</v>
+      </c>
+      <c r="E48" s="59">
+        <v>24</v>
+      </c>
+      <c r="F48" s="59">
+        <v>0.6</v>
+      </c>
+      <c r="G48" s="59">
+        <v>13.4</v>
+      </c>
+      <c r="H48" s="59">
+        <v>51.6</v>
+      </c>
+      <c r="I48" s="59">
+        <v>0.3</v>
+      </c>
+      <c r="J48" s="59">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="55">
+        <v>420</v>
+      </c>
+      <c r="C49" s="57">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D49" s="57">
+        <v>1.23</v>
+      </c>
+      <c r="E49" s="57">
+        <v>18</v>
+      </c>
+      <c r="F49" s="57">
+        <v>0</v>
+      </c>
+      <c r="G49" s="57">
+        <v>3.1</v>
+      </c>
+      <c r="H49" s="57">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="I49" s="57">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J49" s="57">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="55">
+        <v>150</v>
+      </c>
+      <c r="C50" s="57">
+        <v>0.59</v>
+      </c>
+      <c r="D50" s="57">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E50" s="57">
+        <v>8</v>
+      </c>
+      <c r="F50" s="57">
+        <v>0</v>
+      </c>
+      <c r="G50" s="57">
+        <v>14.9</v>
+      </c>
+      <c r="H50" s="57">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="I50" s="57">
+        <v>0</v>
+      </c>
+      <c r="J50" s="57">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="55">
+        <v>150</v>
+      </c>
+      <c r="C51" s="57">
+        <v>0.59</v>
+      </c>
+      <c r="D51" s="57">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E51" s="57">
+        <v>8</v>
+      </c>
+      <c r="F51" s="57">
+        <v>0</v>
+      </c>
+      <c r="G51" s="58"/>
+      <c r="H51" s="57">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="I51" s="57">
+        <v>0</v>
+      </c>
+      <c r="J51" s="57">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="55">
+        <v>180</v>
+      </c>
+      <c r="C52" s="57">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D52" s="57">
+        <v>2.19</v>
+      </c>
+      <c r="E52" s="57">
+        <v>12</v>
+      </c>
+      <c r="F52" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="G52" s="57">
+        <v>3.4</v>
+      </c>
+      <c r="H52" s="57">
+        <v>12.9</v>
+      </c>
+      <c r="I52" s="57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J52" s="57">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" s="55">
+        <v>180</v>
+      </c>
+      <c r="C53" s="57">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D53" s="57">
+        <v>2.19</v>
+      </c>
+      <c r="E53" s="57">
+        <v>12</v>
+      </c>
+      <c r="F53" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="G53" s="57">
+        <v>3.4</v>
+      </c>
+      <c r="H53" s="57">
+        <v>12.9</v>
+      </c>
+      <c r="I53" s="57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J53" s="57">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="55">
+        <v>2800</v>
+      </c>
+      <c r="C54" s="57">
+        <v>3.66</v>
+      </c>
+      <c r="D54" s="57">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="E54" s="57">
+        <v>120</v>
+      </c>
+      <c r="F54" s="57">
+        <v>0</v>
+      </c>
+      <c r="G54" s="57">
+        <v>0</v>
+      </c>
+      <c r="H54" s="57">
+        <v>0.11</v>
+      </c>
+      <c r="I54" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="J54" s="57">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="55">
+        <v>2800</v>
+      </c>
+      <c r="C55" s="57">
+        <v>3.66</v>
+      </c>
+      <c r="D55" s="57">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="E55" s="57">
+        <v>120</v>
+      </c>
+      <c r="F55" s="57">
+        <v>0</v>
+      </c>
+      <c r="G55" s="57">
+        <v>0</v>
+      </c>
+      <c r="H55" s="57">
+        <v>0.11</v>
+      </c>
+      <c r="I55" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="J55" s="57">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="55">
+        <v>2800</v>
+      </c>
+      <c r="C56" s="57">
+        <v>3.66</v>
+      </c>
+      <c r="D56" s="57">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="E56" s="57">
+        <v>120</v>
+      </c>
+      <c r="F56" s="57">
+        <v>0</v>
+      </c>
+      <c r="G56" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="H56" s="57">
+        <v>0.11</v>
+      </c>
+      <c r="I56" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="J56" s="57">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A57" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="55">
+        <v>600</v>
+      </c>
+      <c r="C57" s="57">
+        <v>5</v>
+      </c>
+      <c r="D57" s="57">
+        <v>42.68</v>
+      </c>
+      <c r="E57" s="57">
+        <v>122</v>
+      </c>
+      <c r="F57" s="57">
+        <v>0</v>
+      </c>
+      <c r="G57" s="57">
+        <v>2158.6999999999998</v>
+      </c>
+      <c r="H57" s="57">
+        <v>312.85000000000002</v>
+      </c>
+      <c r="I57" s="57">
+        <v>962.9</v>
+      </c>
+      <c r="J57" s="57">
+        <v>60006</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="55">
+        <v>1000</v>
+      </c>
+      <c r="C58" s="57">
+        <v>3.96</v>
+      </c>
+      <c r="D58" s="57">
+        <v>16.46</v>
+      </c>
+      <c r="E58" s="57">
+        <v>54.3</v>
+      </c>
+      <c r="F58" s="57">
+        <v>0</v>
+      </c>
+      <c r="G58" s="57">
+        <v>23040</v>
+      </c>
+      <c r="H58" s="57">
+        <v>107605.4</v>
+      </c>
+      <c r="I58" s="57">
+        <v>0</v>
+      </c>
+      <c r="J58" s="57">
+        <v>8033.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A59" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="55">
+        <v>1000</v>
+      </c>
+      <c r="C59" s="57">
+        <v>3.96</v>
+      </c>
+      <c r="D59" s="57">
+        <v>16.46</v>
+      </c>
+      <c r="E59" s="57">
+        <v>54.3</v>
+      </c>
+      <c r="F59" s="57">
+        <v>0</v>
+      </c>
+      <c r="G59" s="57">
+        <v>23040</v>
+      </c>
+      <c r="H59" s="57">
+        <v>107605.4</v>
+      </c>
+      <c r="I59" s="57">
+        <v>0</v>
+      </c>
+      <c r="J59" s="57">
+        <v>8033.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A60" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B60" s="55">
+        <v>1000</v>
+      </c>
+      <c r="C60" s="57">
+        <v>3.96</v>
+      </c>
+      <c r="D60" s="57">
+        <v>16.46</v>
+      </c>
+      <c r="E60" s="57">
+        <v>54.3</v>
+      </c>
+      <c r="F60" s="57">
+        <v>0</v>
+      </c>
+      <c r="G60" s="57">
+        <v>23040</v>
+      </c>
+      <c r="H60" s="57">
+        <v>107605.4</v>
+      </c>
+      <c r="I60" s="57">
+        <v>0</v>
+      </c>
+      <c r="J60" s="57">
+        <v>8033.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A61" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" s="55">
+        <v>1200</v>
+      </c>
+      <c r="C61" s="57">
+        <v>3.66</v>
+      </c>
+      <c r="D61" s="57">
+        <v>14.6</v>
+      </c>
+      <c r="E61" s="57">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="F61" s="57">
+        <v>229.86</v>
+      </c>
+      <c r="G61" s="57">
+        <v>5183</v>
+      </c>
+      <c r="H61" s="57">
+        <v>19904.66</v>
+      </c>
+      <c r="I61" s="57">
+        <v>107.7</v>
+      </c>
+      <c r="J61" s="57">
+        <v>1811.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A62" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" s="55">
+        <v>1200</v>
+      </c>
+      <c r="C62" s="57">
+        <v>3.66</v>
+      </c>
+      <c r="D62" s="57">
+        <v>14.6</v>
+      </c>
+      <c r="E62" s="57">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="F62" s="57">
+        <v>229.86</v>
+      </c>
+      <c r="G62" s="57">
+        <v>5183</v>
+      </c>
+      <c r="H62" s="57">
+        <v>19904.66</v>
+      </c>
+      <c r="I62" s="57">
+        <v>107.7</v>
+      </c>
+      <c r="J62" s="57">
+        <v>1811.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A63" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="55">
+        <v>770</v>
+      </c>
+      <c r="C63" s="57">
+        <v>1.01</v>
+      </c>
+      <c r="D63" s="57">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="E63" s="57">
+        <v>33</v>
+      </c>
+      <c r="F63" s="57">
+        <v>0</v>
+      </c>
+      <c r="G63" s="57">
+        <v>0</v>
+      </c>
+      <c r="H63" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="I63" s="57">
+        <v>0.03</v>
+      </c>
+      <c r="J63" s="57">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A64" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" s="55">
+        <v>275</v>
+      </c>
+      <c r="C64" s="57">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D64" s="57">
+        <v>4.53</v>
+      </c>
+      <c r="E64" s="57">
+        <v>15</v>
+      </c>
+      <c r="F64" s="57">
+        <v>0</v>
+      </c>
+      <c r="G64" s="57">
+        <v>1741.5</v>
+      </c>
+      <c r="H64" s="57">
+        <v>8137.76</v>
+      </c>
+      <c r="I64" s="57">
+        <v>0</v>
+      </c>
+      <c r="J64" s="57">
+        <v>608.33000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A65" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B65" s="55">
+        <v>275</v>
+      </c>
+      <c r="C65" s="57">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D65" s="57">
+        <v>4.53</v>
+      </c>
+      <c r="E65" s="57">
+        <v>15</v>
+      </c>
+      <c r="F65" s="57">
+        <v>0</v>
+      </c>
+      <c r="G65" s="57">
+        <v>1741.5</v>
+      </c>
+      <c r="H65" s="57">
+        <v>8137.76</v>
+      </c>
+      <c r="I65" s="57">
+        <v>0</v>
+      </c>
+      <c r="J65" s="57">
+        <v>608.33000000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A66" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="55">
+        <v>330</v>
+      </c>
+      <c r="C66" s="57">
+        <v>1.01</v>
+      </c>
+      <c r="D66" s="57">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E66" s="57">
+        <v>22</v>
+      </c>
+      <c r="F66" s="57">
+        <v>17.38</v>
+      </c>
+      <c r="G66" s="57">
+        <v>392.81</v>
+      </c>
+      <c r="H66" s="57">
+        <v>1505.19</v>
+      </c>
+      <c r="I66" s="57">
+        <v>10.43</v>
+      </c>
+      <c r="J66" s="57">
+        <v>139.05000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A67" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" s="55">
+        <v>330</v>
+      </c>
+      <c r="C67" s="57">
+        <v>1.01</v>
+      </c>
+      <c r="D67" s="57">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E67" s="57">
+        <v>22</v>
+      </c>
+      <c r="F67" s="57">
+        <v>17.38</v>
+      </c>
+      <c r="G67" s="57">
+        <v>392.81</v>
+      </c>
+      <c r="H67" s="57">
+        <v>1505.19</v>
+      </c>
+      <c r="I67" s="57">
+        <v>10.43</v>
+      </c>
+      <c r="J67" s="57">
+        <v>139.05000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A68" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" s="55">
+        <v>168</v>
+      </c>
+      <c r="C68" s="57">
+        <v>0.22</v>
+      </c>
+      <c r="D68" s="57">
+        <v>0.49</v>
+      </c>
+      <c r="E68" s="57">
+        <v>7</v>
+      </c>
+      <c r="F68" s="57"/>
+      <c r="G68" s="57">
+        <v>0</v>
+      </c>
+      <c r="H68" s="57">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="I68" s="57">
+        <v>1E-3</v>
+      </c>
+      <c r="J68" s="57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A69" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69" s="55">
+        <v>60</v>
+      </c>
+      <c r="C69" s="57">
+        <v>0.24</v>
+      </c>
+      <c r="D69" s="57">
+        <v>0.98</v>
+      </c>
+      <c r="E69" s="57">
+        <v>3</v>
+      </c>
+      <c r="F69" s="57"/>
+      <c r="G69" s="57">
+        <v>560.04999999999995</v>
+      </c>
+      <c r="H69" s="57">
+        <v>2602.2399999999998</v>
+      </c>
+      <c r="I69" s="57">
+        <v>0</v>
+      </c>
+      <c r="J69" s="57">
+        <v>209.24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A70" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="55">
+        <v>60</v>
+      </c>
+      <c r="C70" s="57">
+        <v>0.24</v>
+      </c>
+      <c r="D70" s="57">
+        <v>0.98</v>
+      </c>
+      <c r="E70" s="57">
+        <v>3</v>
+      </c>
+      <c r="F70" s="57"/>
+      <c r="G70" s="57">
+        <v>560.04999999999995</v>
+      </c>
+      <c r="H70" s="57">
+        <v>2602.2399999999998</v>
+      </c>
+      <c r="I70" s="57">
+        <v>0</v>
+      </c>
+      <c r="J70" s="57">
+        <v>209.24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A71" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B71" s="55">
+        <v>72</v>
+      </c>
+      <c r="C71" s="57">
+        <v>0.22</v>
+      </c>
+      <c r="D71" s="57">
+        <v>0.88</v>
+      </c>
+      <c r="E71" s="57">
+        <v>5</v>
+      </c>
+      <c r="F71" s="57">
+        <v>1.05</v>
+      </c>
+      <c r="G71" s="57">
+        <v>1.05</v>
+      </c>
+      <c r="H71" s="57">
+        <v>73</v>
+      </c>
+      <c r="I71" s="57">
+        <v>0.35</v>
+      </c>
+      <c r="J71" s="57">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A72" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" s="55">
+        <v>72</v>
+      </c>
+      <c r="C72" s="57">
+        <v>0.22</v>
+      </c>
+      <c r="D72" s="57">
+        <v>0.88</v>
+      </c>
+      <c r="E72" s="57">
+        <v>5</v>
+      </c>
+      <c r="F72" s="57">
+        <v>1.05</v>
+      </c>
+      <c r="G72" s="57">
+        <v>1.05</v>
+      </c>
+      <c r="H72" s="57">
+        <v>73</v>
+      </c>
+      <c r="I72" s="57">
+        <v>0.35</v>
+      </c>
+      <c r="J72" s="57">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A73" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="55">
+        <v>980</v>
+      </c>
+      <c r="C73" s="57">
+        <v>1.28</v>
+      </c>
+      <c r="D73" s="57">
+        <v>2.88</v>
+      </c>
+      <c r="E73" s="57">
+        <v>42</v>
+      </c>
+      <c r="F73" s="57">
+        <v>0</v>
+      </c>
+      <c r="G73" s="57">
+        <v>0</v>
+      </c>
+      <c r="H73" s="57">
+        <v>0.01</v>
+      </c>
+      <c r="I73" s="57">
+        <v>0.03</v>
+      </c>
+      <c r="J73" s="57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A74" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" s="55">
+        <v>19</v>
+      </c>
+      <c r="C74" s="57">
+        <v>350</v>
+      </c>
+      <c r="D74" s="57">
+        <v>1.39</v>
+      </c>
+      <c r="E74" s="57">
+        <v>19</v>
+      </c>
+      <c r="F74" s="57">
+        <v>0</v>
+      </c>
+      <c r="G74" s="57">
+        <v>2930.4</v>
+      </c>
+      <c r="H74" s="57">
+        <v>13678.8</v>
+      </c>
+      <c r="I74" s="57">
+        <v>0</v>
+      </c>
+      <c r="J74" s="57">
+        <v>983.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A75" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75" s="55">
+        <v>19</v>
+      </c>
+      <c r="C75" s="58"/>
+      <c r="D75" s="57">
+        <v>1.39</v>
+      </c>
+      <c r="E75" s="57">
+        <v>19</v>
+      </c>
+      <c r="F75" s="57">
+        <v>0</v>
+      </c>
+      <c r="G75" s="58"/>
+      <c r="H75" s="57">
+        <v>13678.8</v>
+      </c>
+      <c r="I75" s="57">
+        <v>0</v>
+      </c>
+      <c r="J75" s="57">
+        <v>983.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A76" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B76" s="55">
+        <v>420</v>
+      </c>
+      <c r="C76" s="57">
+        <v>1.28</v>
+      </c>
+      <c r="D76" s="57">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E76" s="57">
+        <v>28</v>
+      </c>
+      <c r="F76" s="57">
+        <v>31.28</v>
+      </c>
+      <c r="G76" s="57">
+        <v>636.14</v>
+      </c>
+      <c r="H76" s="57">
+        <v>2436.81</v>
+      </c>
+      <c r="I76" s="57">
+        <v>13.9</v>
+      </c>
+      <c r="J76" s="57">
+        <v>222.48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A77" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B77" s="55">
+        <v>420</v>
+      </c>
+      <c r="C77" s="57">
+        <v>1.28</v>
+      </c>
+      <c r="D77" s="57">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E77" s="57">
+        <v>28</v>
+      </c>
+      <c r="F77" s="57">
+        <v>31.28</v>
+      </c>
+      <c r="G77" s="57">
+        <v>636.14</v>
+      </c>
+      <c r="H77" s="57">
+        <v>2436.81</v>
+      </c>
+      <c r="I77" s="57">
+        <v>13.9</v>
+      </c>
+      <c r="J77" s="57">
+        <v>222.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>